<commit_message>
Great Circle Calculations Added
</commit_message>
<xml_diff>
--- a/Lab3/Q4.xlsx
+++ b/Lab3/Q4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lostk\OneDrive\Desktop\Working Directory\Schule\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBA60BEC-822E-4040-9386-A457BEA0193D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863D13AF-7C82-49E3-8B61-B81E2A7013B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2265" windowWidth="18660" windowHeight="11775" xr2:uid="{BA8E1863-1EF9-4B1A-AEA0-B0BDF4E29E69}"/>
+    <workbookView xWindow="4560" yWindow="375" windowWidth="18660" windowHeight="11775" xr2:uid="{BA8E1863-1EF9-4B1A-AEA0-B0BDF4E29E69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Top-Left Corner</t>
   </si>
@@ -49,14 +71,34 @@
   </si>
   <si>
     <t>Radius of Earth (km):</t>
+  </si>
+  <si>
+    <t>Lat_Rad</t>
+  </si>
+  <si>
+    <t>Long_Rad</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,27 +443,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4398F4-BDB9-4860-8A40-DA8C43B1F1E7}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -430,8 +486,24 @@
       <c r="C2">
         <v>-138.70099999999999</v>
       </c>
+      <c r="D2">
+        <f>RADIANS(B2)</f>
+        <v>1.1351097856195522</v>
+      </c>
+      <c r="E2" cm="1">
+        <f t="array" ref="E2:E3">RADIANS(C2:C3)</f>
+        <v>-2.4207891258086551</v>
+      </c>
+      <c r="F2">
+        <f>E3-E2</f>
+        <v>-0.17238617021947977</v>
+      </c>
+      <c r="G2" s="1">
+        <f>ACOS(SIN(D2)*SIN(D3)+COS(D2)*COS(D3)*COS(F2))*B5</f>
+        <v>592.56230575279665</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -441,8 +513,15 @@
       <c r="C3">
         <v>-148.578</v>
       </c>
+      <c r="D3">
+        <f>RADIANS(B3)</f>
+        <v>1.1991633691677439</v>
+      </c>
+      <c r="E3">
+        <v>-2.5931752960281349</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -452,5 +531,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>